<commit_message>
JLCpcb production files ready for CV rev 2
</commit_message>
<xml_diff>
--- a/kicad_v2/gerber/veloce-top-pos.xlsx
+++ b/kicad_v2/gerber/veloce-top-pos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="85">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -64,6 +64,39 @@
     <t xml:space="preserve">D8</t>
   </si>
   <si>
+    <t xml:space="preserve">D9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D19</t>
+  </si>
+  <si>
     <t xml:space="preserve">Q1</t>
   </si>
   <si>
@@ -88,6 +121,30 @@
     <t xml:space="preserve">Q8</t>
   </si>
   <si>
+    <t xml:space="preserve">Q9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q16</t>
+  </si>
+  <si>
     <t xml:space="preserve">R1</t>
   </si>
   <si>
@@ -173,6 +230,51 @@
   </si>
   <si>
     <t xml:space="preserve">R29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R48</t>
   </si>
 </sst>
 </file>
@@ -187,6 +289,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -272,15 +375,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.02"/>
   </cols>
   <sheetData>
@@ -306,10 +409,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>15</v>
+        <v>-37.5</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -323,10 +426,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>15</v>
+        <v>-37.5</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -340,10 +443,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>15</v>
+        <v>-37.5</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -357,10 +460,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>15</v>
+        <v>-37.5</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -374,10 +477,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>15</v>
+        <v>-37.5</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
@@ -391,10 +494,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>15</v>
+        <v>-37.5</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>37</v>
+        <v>-7</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -408,10 +511,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>15</v>
+        <v>-37.5</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>27</v>
+        <v>-17</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
@@ -425,10 +528,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>15</v>
+        <v>-37.5</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>17</v>
+        <v>-27</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
@@ -442,16 +545,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>22.5</v>
+        <v>-33</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>87</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,16 +562,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>22.5</v>
+        <v>-33</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,16 +579,16 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>19.5</v>
+        <v>-33</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,16 +596,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>19.5</v>
+        <v>-33</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,16 +613,16 @@
         <v>18</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>19.5</v>
+        <v>-33</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,16 +630,16 @@
         <v>19</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>19.5</v>
+        <v>-33</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>37</v>
+        <v>-9</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,16 +647,16 @@
         <v>20</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>19.5</v>
+        <v>-33</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>27</v>
+        <v>-19</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,16 +664,16 @@
         <v>21</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>19.5</v>
+        <v>-33</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>17</v>
+        <v>-29</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -578,16 +681,16 @@
         <v>22</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>31.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>84.5</v>
+        <v>-33.5</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,16 +698,16 @@
         <v>23</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>31.5</v>
+        <v>-21</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>74.5</v>
+        <v>-33.5</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,16 +715,16 @@
         <v>24</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>31.5</v>
+        <v>-39</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>89.5</v>
+        <v>-33.5</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,16 +732,16 @@
         <v>25</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>31.5</v>
+        <v>-26</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>79.5</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,16 +749,16 @@
         <v>26</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>23.5</v>
+        <v>-17.5</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -663,16 +766,16 @@
         <v>27</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>23.5</v>
+        <v>-26</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,16 +783,16 @@
         <v>28</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>23.5</v>
+        <v>-17.5</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,16 +800,16 @@
         <v>29</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>23.5</v>
+        <v>-26</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,16 +817,16 @@
         <v>30</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>23.5</v>
+        <v>-17.5</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,16 +834,16 @@
         <v>31</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>23.5</v>
+        <v>-26</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -748,16 +851,16 @@
         <v>32</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>23.5</v>
+        <v>-17.5</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,16 +868,16 @@
         <v>33</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>23.5</v>
+        <v>-26</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,16 +885,16 @@
         <v>34</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>23.5</v>
+        <v>-17.5</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -799,16 +902,16 @@
         <v>35</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>23.5</v>
+        <v>-26</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>16</v>
+        <v>-7</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -816,16 +919,16 @@
         <v>36</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>23.5</v>
+        <v>-17.5</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>28</v>
+        <v>-9</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,16 +936,16 @@
         <v>37</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>23.5</v>
+        <v>-26</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>18</v>
+        <v>-17</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,16 +953,16 @@
         <v>38</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>59.29</v>
+        <v>-17.5</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>87</v>
+        <v>-19</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,16 +970,16 @@
         <v>39</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>59.29</v>
+        <v>-26</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>84</v>
+        <v>-27</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,16 +987,16 @@
         <v>40</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>70.29</v>
+        <v>-17.5</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>87</v>
+        <v>-29</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,16 +1004,16 @@
         <v>41</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>70.29</v>
+        <v>-17.5</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>84</v>
+        <v>45.5</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,16 +1021,16 @@
         <v>42</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>83.81</v>
+        <v>-17.5</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>14.5</v>
+        <v>43.3</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -935,10 +1038,10 @@
         <v>43</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>83.81</v>
+        <v>-17.5</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>89.5</v>
+        <v>39</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>6</v>
@@ -952,16 +1055,16 @@
         <v>44</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>83.81</v>
+        <v>-17.5</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>79.5</v>
+        <v>35.5</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -969,16 +1072,16 @@
         <v>45</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>83.81</v>
+        <v>-17.5</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>69.5</v>
+        <v>33</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -986,10 +1089,10 @@
         <v>46</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>83.81</v>
+        <v>-17.5</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>59.5</v>
+        <v>29</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>6</v>
@@ -1003,16 +1106,16 @@
         <v>47</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>83.81</v>
+        <v>-17.5</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>49.5</v>
+        <v>25.5</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,16 +1123,16 @@
         <v>48</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>83.81</v>
+        <v>-17.5</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>39.5</v>
+        <v>23</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1037,10 +1140,10 @@
         <v>49</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>83.81</v>
+        <v>-17.5</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>29.5</v>
+        <v>19</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>6</v>
@@ -1054,16 +1157,594 @@
         <v>50</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>83.81</v>
+        <v>-17.5</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>19.5</v>
+        <v>15.5</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E46" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="1" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>-7</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>-11</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>-14.5</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>-17</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>-21</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>-24.5</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>-27</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="1" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>-31</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="1" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="1" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="1" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" s="1" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>-7.5</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66" s="1" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67" s="1" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>-23.7</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="1" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="C68" s="1" t="n">
+        <v>-27.7</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" s="1" t="n">
+        <v>36.51</v>
+      </c>
+      <c r="C69" s="1" t="n">
+        <v>-31.7</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="C70" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="C72" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="C73" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>-5</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>-15</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>-25</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78" s="1" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>-37</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79" s="1" t="n">
+        <v>-21</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>-37</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80" s="1" t="n">
+        <v>-39</v>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>-37</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" s="1" t="n">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>